<commit_message>
Revert "fix bug kwr003-07-04"
This reverts commit 9269d03bcaddbf42ca4d865324fd004544df3864.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR007_template.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR007_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="20376" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="振休確認表(日数管理_紐付あり_年月日) (2)" sheetId="4" r:id="rId1"/>
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'振休確認表(日数管理_紐付あり_年月日)'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'振休確認表(日数管理_紐付あり_年月日) (2)'!#REF!</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'振休確認表(日数管理_紐付あり_年月日)'!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'振休確認表(日数管理_紐付あり_年月日) (2)'!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -516,6 +517,36 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -525,38 +556,8 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -842,28 +843,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.375" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.33203125" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="6" customWidth="1"/>
-    <col min="2" max="9" width="6.375" style="6"/>
-    <col min="10" max="19" width="6.375" style="7"/>
-    <col min="20" max="20" width="6.375" style="9"/>
-    <col min="21" max="21" width="6.375" style="6" customWidth="1"/>
-    <col min="22" max="16384" width="6.375" style="6"/>
+    <col min="1" max="1" width="13.77734375" style="6" customWidth="1"/>
+    <col min="2" max="9" width="6.33203125" style="6"/>
+    <col min="10" max="19" width="6.33203125" style="7"/>
+    <col min="20" max="20" width="6.33203125" style="9"/>
+    <col min="21" max="21" width="6.33203125" style="6" customWidth="1"/>
+    <col min="22" max="16384" width="6.33203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -880,122 +881,122 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="35"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="29"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="30"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="35"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="29"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="30"/>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1">
-      <c r="A4" s="35"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="27"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="35"/>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="27"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="35"/>
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1018,7 +1019,7 @@
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3"/>
@@ -1041,7 +1042,7 @@
       <c r="U8" s="3"/>
     </row>
     <row r="9" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
@@ -1064,7 +1065,7 @@
       <c r="U9" s="5"/>
     </row>
     <row r="10" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
@@ -1087,7 +1088,7 @@
       <c r="U10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -1110,7 +1111,7 @@
       <c r="U11" s="10"/>
     </row>
     <row r="12" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A12" s="24"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
@@ -1133,7 +1134,7 @@
       <c r="U12" s="3"/>
     </row>
     <row r="13" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
@@ -1156,7 +1157,7 @@
       <c r="U13" s="5"/>
     </row>
     <row r="14" spans="1:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A14" s="31"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
@@ -1179,7 +1180,7 @@
       <c r="U14" s="13"/>
     </row>
     <row r="15" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A15" s="32"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1202,7 +1203,7 @@
       <c r="U15" s="16"/>
     </row>
     <row r="16" spans="1:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A16" s="33"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20" t="s">
@@ -1299,6 +1300,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A6:U6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="M2:M3"/>
@@ -1315,38 +1348,6 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="A6:U6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
@@ -1361,15 +1362,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.375" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.33203125" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="6" customWidth="1"/>
-    <col min="2" max="9" width="6.375" style="6"/>
-    <col min="10" max="19" width="6.375" style="7"/>
-    <col min="20" max="20" width="6.375" style="9"/>
-    <col min="21" max="16384" width="6.375" style="6"/>
+    <col min="1" max="1" width="13.77734375" style="6" customWidth="1"/>
+    <col min="2" max="9" width="6.33203125" style="6"/>
+    <col min="10" max="19" width="6.33203125" style="7"/>
+    <col min="20" max="20" width="6.33203125" style="9"/>
+    <col min="21" max="16384" width="6.33203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="13.5" customHeight="1">
@@ -1611,7 +1612,7 @@
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "fix bug kwr003-07-04""
This reverts commit 1fe56266285b6a482aaf3c89e1a1e2b4770b5913.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR007_template.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR007_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20376" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="振休確認表(日数管理_紐付あり_年月日) (2)" sheetId="4" r:id="rId1"/>
@@ -13,7 +13,6 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'振休確認表(日数管理_紐付あり_年月日)'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'振休確認表(日数管理_紐付あり_年月日) (2)'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'振休確認表(日数管理_紐付あり_年月日)'!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'振休確認表(日数管理_紐付あり_年月日) (2)'!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -517,9 +516,33 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -529,35 +552,11 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -843,28 +842,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.33203125" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.375" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="6" customWidth="1"/>
-    <col min="2" max="9" width="6.33203125" style="6"/>
-    <col min="10" max="19" width="6.33203125" style="7"/>
-    <col min="20" max="20" width="6.33203125" style="9"/>
-    <col min="21" max="21" width="6.33203125" style="6" customWidth="1"/>
-    <col min="22" max="16384" width="6.33203125" style="6"/>
+    <col min="1" max="1" width="13.75" style="6" customWidth="1"/>
+    <col min="2" max="9" width="6.375" style="6"/>
+    <col min="10" max="19" width="6.375" style="7"/>
+    <col min="20" max="20" width="6.375" style="9"/>
+    <col min="21" max="21" width="6.375" style="6" customWidth="1"/>
+    <col min="22" max="16384" width="6.375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -881,122 +880,122 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="30"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="30"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="29"/>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1">
-      <c r="A4" s="28"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="35"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="27"/>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1">
-      <c r="A5" s="28"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="35"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="27"/>
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A7" s="33"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1019,7 +1018,7 @@
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A8" s="34"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3"/>
@@ -1042,7 +1041,7 @@
       <c r="U8" s="3"/>
     </row>
     <row r="9" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A9" s="22"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
@@ -1065,7 +1064,7 @@
       <c r="U9" s="5"/>
     </row>
     <row r="10" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A10" s="22"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
@@ -1088,7 +1087,7 @@
       <c r="U10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A11" s="33"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -1111,7 +1110,7 @@
       <c r="U11" s="10"/>
     </row>
     <row r="12" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A12" s="34"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
@@ -1134,7 +1133,7 @@
       <c r="U12" s="3"/>
     </row>
     <row r="13" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A13" s="22"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
@@ -1157,7 +1156,7 @@
       <c r="U13" s="5"/>
     </row>
     <row r="14" spans="1:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
@@ -1180,7 +1179,7 @@
       <c r="U14" s="13"/>
     </row>
     <row r="15" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A15" s="24"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1203,7 +1202,7 @@
       <c r="U15" s="16"/>
     </row>
     <row r="16" spans="1:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20" t="s">
@@ -1300,6 +1299,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
     <mergeCell ref="A6:U6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
@@ -1316,38 +1347,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
@@ -1362,15 +1361,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.33203125" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.375" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="6" customWidth="1"/>
-    <col min="2" max="9" width="6.33203125" style="6"/>
-    <col min="10" max="19" width="6.33203125" style="7"/>
-    <col min="20" max="20" width="6.33203125" style="9"/>
-    <col min="21" max="16384" width="6.33203125" style="6"/>
+    <col min="1" max="1" width="13.75" style="6" customWidth="1"/>
+    <col min="2" max="9" width="6.375" style="6"/>
+    <col min="10" max="19" width="6.375" style="7"/>
+    <col min="20" max="20" width="6.375" style="9"/>
+    <col min="21" max="16384" width="6.375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="13.5" customHeight="1">
@@ -1612,7 +1611,7 @@
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>